<commit_message>
updates excel file from server
</commit_message>
<xml_diff>
--- a/Lernjournalsbewertung.xlsx
+++ b/Lernjournalsbewertung.xlsx
@@ -1,31 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbhishekGupta\Desktop\Abhishek Gupta_MPM\Entwicklungs methoden Für Nachhaltige Produkte\Preperation_Vorlessung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mpm-data\mpm\Lehre\Vorlesungen\Entwicklungsmethoden_fuer_nachhaltige_Produkte\Bewertungskriterium\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E2B4D1D-B356-2849-8E3F-4B9D86D8B5A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournalsbewertung" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
+    <sheet name="Bewertungskriterium" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gupta, Abhishek</author>
+  </authors>
+  <commentList>
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gupta, Abhishek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+11 = 10</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
   <si>
     <t>Matrikelnr.</t>
   </si>
@@ -66,18 +110,6 @@
     <t>Dokumentation/ Ergebnis</t>
   </si>
   <si>
-    <t>0-4</t>
-  </si>
-  <si>
-    <t>5-6</t>
-  </si>
-  <si>
-    <t>7-8</t>
-  </si>
-  <si>
-    <t>9-10</t>
-  </si>
-  <si>
     <t>Arbeitsziel z.T. übertroffen</t>
   </si>
   <si>
@@ -228,32 +260,74 @@
     <t>Pkt. P2</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Group Nr.</t>
-  </si>
-  <si>
-    <t>Lernjournal Punkte</t>
-  </si>
-  <si>
-    <t>Projektarbeit Punkte</t>
-  </si>
-  <si>
-    <t>Average</t>
+    <t>Criteria</t>
+  </si>
+  <si>
+    <t>Display of Graphic/ Results/ Tables/ Examples</t>
+  </si>
+  <si>
+    <t>Transfer &amp; Reflection</t>
+  </si>
+  <si>
+    <t>Understanding The Concept Of Lernjournal</t>
+  </si>
+  <si>
+    <t>The topics that are discussed in the lectures are to be explained</t>
+  </si>
+  <si>
+    <t>The explanation just does not have to be a copy paste of the things taught in lectures</t>
+  </si>
+  <si>
+    <t>If used any table, graphics etc. a proper explanation is expected</t>
+  </si>
+  <si>
+    <t>The structure can be either a scientific paper or a completely creative format, but constant</t>
+  </si>
+  <si>
+    <t>The topics and sub-topics to be explained in proper sequence or not to be skipped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The transfer means the usage of the knowledge in various ways to be shown in other parts of the lectures. </t>
+  </si>
+  <si>
+    <t>Combination of theory and praxis examples</t>
+  </si>
+  <si>
+    <t>Explanation of the Topics in a way which shows that the student has understood, also with unanswered questions</t>
+  </si>
+  <si>
+    <t>Explaining what has been understood and what has been left unanswered or what has been understood in adifferent way as sompared to taught</t>
+  </si>
+  <si>
+    <t>The Lernjournal is to show that the students have understood the lectures in such a way that they can elaborate on the topics in their own language and also parallel use the resources with an understanding. A regular students Journal will be complete with extra examples from and outside the lectures, as compared to an irregular students, the Journals will be just bullet points</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>8-9</t>
+  </si>
+  <si>
+    <t>8-10</t>
+  </si>
+  <si>
+    <t>Independent of the format used, no citation is acceptable</t>
+  </si>
+  <si>
+    <t>0-3</t>
+  </si>
+  <si>
+    <t>4-5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,6 +365,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -317,7 +404,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -667,6 +754,34 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -681,7 +796,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -755,9 +870,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -776,26 +888,51 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -817,14 +954,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Gut" xfId="2" builtinId="26"/>
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Stil 1" xfId="3"/>
-    <cellStyle name="Stil 2" xfId="4"/>
+    <cellStyle name="Stil 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Stil 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -1173,40 +1313,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="50" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" customWidth="1"/>
-    <col min="9" max="9" width="52.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" customWidth="1"/>
-    <col min="17" max="17" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.32421875" customWidth="1"/>
+    <col min="3" max="3" width="39.4140625" customWidth="1"/>
+    <col min="4" max="4" width="11.56640625" customWidth="1"/>
+    <col min="5" max="5" width="50.04296875" customWidth="1"/>
+    <col min="7" max="7" width="42.375" customWidth="1"/>
+    <col min="9" max="9" width="52.73046875" customWidth="1"/>
+    <col min="11" max="11" width="18.16015625" customWidth="1"/>
+    <col min="13" max="13" width="12.10546875" customWidth="1"/>
+    <col min="15" max="15" width="13.1796875" customWidth="1"/>
+    <col min="17" max="17" width="32.8203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="44"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="52"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1214,27 +1354,27 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="20"/>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -1270,10 +1410,10 @@
         <v>9</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>10</v>
@@ -1283,147 +1423,147 @@
       </c>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:17" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="47" t="s">
+    <row r="9" spans="1:17" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="55" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="28" t="s">
+      <c r="J9" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="34">
-        <v>11</v>
-      </c>
-      <c r="M9" s="30">
-        <v>10</v>
-      </c>
-      <c r="N9" s="31">
-        <v>10</v>
-      </c>
-      <c r="O9" s="32">
-        <v>0.5</v>
+      <c r="L9" s="33">
+        <v>10</v>
+      </c>
+      <c r="M9" s="29">
+        <v>10</v>
+      </c>
+      <c r="N9" s="30">
+        <v>10</v>
+      </c>
+      <c r="O9" s="31">
+        <v>2.5</v>
       </c>
       <c r="P9" s="23">
         <f>((M9+N9)/2)*O9</f>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="Q9" s="6"/>
     </row>
-    <row r="10" spans="1:17" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
+    <row r="10" spans="1:17" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="56"/>
       <c r="B10" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="33" t="s">
+      <c r="J10" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="K10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="34">
-        <v>11</v>
-      </c>
-      <c r="M10" s="30">
-        <v>10</v>
-      </c>
-      <c r="N10" s="30">
+      <c r="L10" s="33">
+        <v>10</v>
+      </c>
+      <c r="M10" s="29">
+        <v>10</v>
+      </c>
+      <c r="N10" s="29">
         <v>10</v>
       </c>
       <c r="O10" s="24">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="P10" s="23">
         <f t="shared" ref="P10:P16" si="0">((M10+N10)/2)*O10</f>
+        <v>15</v>
+      </c>
+      <c r="Q10" s="6"/>
+    </row>
+    <row r="11" spans="1:17" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="56"/>
+      <c r="B11" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="Q10" s="6"/>
-    </row>
-    <row r="11" spans="1:17" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="48"/>
-      <c r="B11" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="34">
-        <v>11</v>
-      </c>
-      <c r="M11" s="30">
-        <v>10</v>
-      </c>
-      <c r="N11" s="30">
+      <c r="L11" s="33">
+        <v>10</v>
+      </c>
+      <c r="M11" s="29">
+        <v>10</v>
+      </c>
+      <c r="N11" s="29">
         <v>10</v>
       </c>
       <c r="O11" s="24">
@@ -1435,241 +1575,249 @@
       </c>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
+    <row r="12" spans="1:17" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="56"/>
       <c r="B12" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="33" t="s">
+      <c r="J12" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="34">
-        <v>11</v>
-      </c>
-      <c r="M12" s="30">
-        <v>10</v>
-      </c>
-      <c r="N12" s="30">
+      <c r="L12" s="33">
+        <v>10</v>
+      </c>
+      <c r="M12" s="29">
+        <v>10</v>
+      </c>
+      <c r="N12" s="29">
         <v>10</v>
       </c>
       <c r="O12" s="24">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="P12" s="23">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:17" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
+    <row r="13" spans="1:17" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="57"/>
       <c r="B13" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="35" t="s">
+      <c r="F13" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="34">
-        <v>11</v>
-      </c>
-      <c r="M13" s="37">
-        <v>10</v>
-      </c>
-      <c r="N13" s="37">
+      <c r="L13" s="33">
+        <v>10</v>
+      </c>
+      <c r="M13" s="35">
+        <v>10</v>
+      </c>
+      <c r="N13" s="35">
         <v>10</v>
       </c>
       <c r="O13" s="26">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="P13" s="23">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14" spans="1:17" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="s">
-        <v>18</v>
+    <row r="14" spans="1:17" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="55" t="s">
+        <v>14</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D14" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="J14" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14" s="16"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="38">
-        <v>10</v>
-      </c>
-      <c r="N14" s="38">
-        <v>10</v>
-      </c>
-      <c r="O14" s="39">
-        <v>2</v>
+      <c r="L14" s="49">
+        <v>10</v>
+      </c>
+      <c r="M14" s="36">
+        <v>10</v>
+      </c>
+      <c r="N14" s="36">
+        <v>10</v>
+      </c>
+      <c r="O14" s="37">
+        <v>1</v>
       </c>
       <c r="P14" s="23">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15" spans="1:17" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
+    <row r="15" spans="1:17" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="57"/>
       <c r="B15" s="26" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="J15" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="40"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37">
-        <v>10</v>
-      </c>
-      <c r="N15" s="37">
+      <c r="L15" s="50">
+        <v>10</v>
+      </c>
+      <c r="M15" s="35">
+        <v>10</v>
+      </c>
+      <c r="N15" s="35">
         <v>10</v>
       </c>
       <c r="O15" s="26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P15" s="23">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:17" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L16" s="34">
-        <v>11</v>
-      </c>
-      <c r="M16" s="42">
-        <v>10</v>
-      </c>
-      <c r="N16" s="42">
+      <c r="L16" s="33">
+        <v>10</v>
+      </c>
+      <c r="M16" s="39">
+        <v>10</v>
+      </c>
+      <c r="N16" s="39">
         <v>10</v>
       </c>
       <c r="O16" s="27">
@@ -1681,7 +1829,7 @@
       </c>
       <c r="Q16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="O17">
         <f>SUM(O9:O16)</f>
@@ -1693,7 +1841,7 @@
       </c>
       <c r="Q17" s="6"/>
     </row>
-    <row r="18" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1722,7 +1870,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1740,7 +1888,7 @@
       <c r="O19" s="9"/>
       <c r="Q19" s="6"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1751,7 +1899,7 @@
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="O20" s="12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="P20" s="13">
         <v>100</v>
@@ -1764,7 +1912,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1780,19 +1928,18 @@
         <v>4</v>
       </c>
       <c r="P21" s="15">
-        <f>0.5*P20</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="Q21" s="14">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R21" s="15">
         <f>0.5*R20</f>
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -1806,19 +1953,18 @@
         <v>3.7</v>
       </c>
       <c r="P22" s="15">
-        <f>0.55*P20</f>
-        <v>55.000000000000007</v>
+        <v>45</v>
       </c>
       <c r="Q22" s="14">
         <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
       <c r="R22" s="15">
         <f>0.55*R20</f>
         <v>27.500000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1834,19 +1980,18 @@
         <v>3.3</v>
       </c>
       <c r="P23" s="15">
-        <f>0.6*P20</f>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="Q23" s="14">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="R23" s="15">
         <f>0.6*R20</f>
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1862,19 +2007,18 @@
         <v>3</v>
       </c>
       <c r="P24" s="15">
-        <f>0.65*P20</f>
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="Q24" s="14">
         <f t="shared" si="1"/>
-        <v>0.65</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R24" s="15">
         <f>0.65*R20</f>
         <v>32.5</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1890,19 +2034,18 @@
         <v>2.7</v>
       </c>
       <c r="P25" s="15">
-        <f>0.7*P20</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="Q25" s="14">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="R25" s="15">
         <f>0.7*R20</f>
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1918,19 +2061,18 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="P26" s="15">
-        <f>0.75*P20</f>
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="Q26" s="14">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="R26" s="15">
         <f>0.75*R20</f>
         <v>37.5</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1946,19 +2088,18 @@
         <v>2</v>
       </c>
       <c r="P27" s="15">
-        <f>0.8*P20</f>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="Q27" s="14">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="R27" s="15">
         <f>0.8*R20</f>
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -1974,19 +2115,18 @@
         <v>1.7</v>
       </c>
       <c r="P28" s="15">
-        <f>0.85*P20</f>
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="Q28" s="14">
         <f t="shared" si="1"/>
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="R28" s="15">
         <f>0.85*R20</f>
         <v>42.5</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -2002,19 +2142,18 @@
         <v>1.3</v>
       </c>
       <c r="P29" s="15">
-        <f>0.9*P20</f>
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="Q29" s="14">
         <f t="shared" si="1"/>
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="R29" s="15">
         <f>0.9*R20</f>
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -2030,12 +2169,11 @@
         <v>1</v>
       </c>
       <c r="P30" s="15">
-        <f>0.95*P20</f>
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="Q30" s="14">
         <f>P30/P$20</f>
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="R30" s="15">
         <f>0.95*R20</f>
@@ -2082,45 +2220,122 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.015625" customWidth="1"/>
+    <col min="2" max="2" width="102.1015625" customWidth="1"/>
+    <col min="4" max="4" width="27.98046875" customWidth="1"/>
+    <col min="5" max="5" width="27.3046875" customWidth="1"/>
+    <col min="6" max="6" width="22.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="58"/>
+      <c r="B7" s="48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58"/>
+      <c r="B8" s="47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="29.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="58"/>
+      <c r="B9" s="46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="E1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" t="s">
-        <v>72</v>
+    </row>
+    <row r="12" spans="1:2" ht="55.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:A9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>